<commit_message>
v2 add find elements
</commit_message>
<xml_diff>
--- a/output2.xlsx
+++ b/output2.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -431,23 +431,23 @@
         <is>
           <t xml:space="preserve">
 "Time Park" - уникальный банный комплекс,  расположенный в районе Москвы Выхино-Жулебино.  "Taim Park" сочетает в себе традиции русского парения с Wellness &amp; Spa.  Это закрытая территория в лесопарковой зоне (800 кв. м),  современный сьют с открытой террасой и камином с живым огнём,  вокруг которого можно посидеть на мягких подушках,  чан с душистыми травами и купель с отделкой из шунгита.  В комплексе с комфортом расположится компания до 12  человек.  Всем гостям предлагаем коллективный аромопар в подарок!
-"Time Park" это:
-- профессиональная парная облицована пихтой,  с подогреваемым полом и мощной дровяной печью;
-- открытая терраса с камином и местами для отдыха;
-- чан с душистыми травами на открытом воздухе;
-- купель с отделкой из целебного шунгита и греческого мрамора на террасе;
-- душевые,  обливная кадушка;
-- услуги пармейстера (помывки,  парения);
-- спа процедуры (массажи,  пилинги,  обёртывания);
+"Time Park" это:
+- профессиональная парная облицована пихтой,  с подогреваемым полом и мощной дровяной печью;
+- открытая терраса с камином и местами для отдыха;
+- чан с душистыми травами на открытом воздухе;
+- купель с отделкой из целебного шунгита и греческого мрамора на террасе;
+- душевые,  обливная кадушка;
+- услуги пармейстера (помывки,  парения);
+- спа процедуры (массажи,  пилинги,  обёртывания);
 - барное меню,  и блюда от шеф-повара. 
-Не допускается приносить свою еду,  так как в нашем комплексе наивкуснейшая кухня и чудесный шеф-повар! Спиртное приносить можно при наличии чека из магазина,  пиво не допускается.  У нас большой выбор пива на любой вкус!
+Не допускается приносить свою еду,  так как в нашем комплексе наивкуснейшая кухня и чудесный шеф-повар! Спиртное приносить можно при наличии чека из магазина,  пиво не допускается.  У нас большой выбор пива на любой вкус!
 Узнать дополнительную информацию или забронировать время посещения можете по телефону: 
-+7 985 795 07 56 
++7 985 795 07 56 
 или на официальном сайте банного комплекса "Time Park":
 https://time-park.ru/
-За сутки: 106
-За последние 30 дней: 216
-Всего: 2346
+За сутки: 226
+За последние 30 дней: 336
+Всего: 2466
 </t>
         </is>
       </c>
@@ -460,158 +460,16 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>СТОИМОСТЬ:
+          <t>СТОИМОСТЬ:
 Минимальное время аренды 2 часа.
-10-00 – 17-00 – 2900 руб/час
+10-00 – 17-00 – 2900 руб/час
 17-00 – 09-00 – 4500 руб/час
-Стоимость указана на компанию до 8 человек, каждый дополнительный человек 500 руб/час.
-Внимание! АКЦИИ:
-- Скидка в честь дня рождения 20% на аренду сьюта, 3 дня до и 3 дня после дня рождения.
-Дополнительно:
-Чан с душистыми травами: 5000 – 8000 руб;
-Услуги пармейстера: 900 – 3500 руб;
-Пилинги: 800 руб;
-Массажи: 1200 – 3500 руб;
-Обёртывания: 1900 руб;
-Маски для лица: 1000 руб/20 мин.
-Продажа:
-Банная шапка TIME PARK (белая/черная) - 750 руб;
-Тапочки резиновые «кроксы» - 600 руб.
-Аренда:
-Простыня – 250 руб;
-Полотенце – 300 руб;
-Халат – 500 руб;
-Веники в ассортименте – 450 руб;
-Веничек травяной ароматный – 250 руб;
-Мешок травяной для чана – 500 руб;
-Вязанка дров для патио – 1000 руб;
-Лыко – 300 руб;
-Мыло – 200 руб;
-Зубной набор – 200 руб;
-Бритвенный набор – 200 руб;
-Уборка парной – 1000 руб. (при самостоятельном парении, с использованием веников, скрабов и т п, без услуг нашего банщика)</t>
+Стоимость указана на компанию до 8 человек, каждый до</t>
         </is>
       </c>
       <c r="E1" t="b">
         <v>0</v>
       </c>
-      <c r="F1" t="inlineStr"/>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>г. Долгопрудный, 3-я Северная линия, дом 2</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Общественная баня.  
-Северные бани в Долгопрудном - это новые общественные бани,  вместимостью до 50 человек.  Баня расположена в Северном районе,  и открыта ежедневно до 23 часов.  
-В бане для гостей:
-- Современная раздевалка,  оборудованная индивидуальными шкафчиками с электронными замками. 
-- Общий зал разделенный на кабинки с комфортными диванами и столом.  В некоторых кабинках есть телевизор. 
-- Своя кухня на территории бани и бар с прохладительными напитками. 
-- Вместительная парная отделана липой.  Огромная печь из 6 тонн чугуна и профессиональные банщики.  Ежечасно банные мастера готовят ароматный пар,  добавляя эвкалипт,  чеснок,  донник и другие травы. 
-- Бассейн,  обливные кадушки и душевые. 
-- Услуги парения,  мойки и массажа. 
-Баня работает ежедневно.  Женский день - вторник. 
-Узнать дополнительную информацию можно по телефону администратора: 
-8 495 665 25 58
-За сутки: 87
-За последние 30 дней: 373
-Всего: 4327
-</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Вид парной: русская баня, русская на дровахКухня: бар, разливное пиво, кафеУслуги: веники, банщик, спа-терапия, оздоровительный массаж, ароматерапия, оплата картамиСервис: бассейн, кондиционер, холодная купель, спутниковое тв, обливное ведро, большой TV, настольные игры
-</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>СТОИМОСТЬ:
-Посещение бани 2 часа - 1000 руб.
-Доплата за последующий час - 300 руб.
-Дети до 7 лет- бесплатно
-Дети с 7 до 14 лет- 500 руб.
-Льготные категории граждан: пенсионеры, ветераны, инвалиды, многодетные семьи - вт, ср, чт ( при входе до 14-00) - 500 руб.
-Доплата за последующий час для льготных категорий граждан - 150 руб.
-Услуги парения и массажа 600 - 2500 руб
-Режим работы: 
-Пн: с 15-00 до 23-00 ч.
-Вт, Ср, Чт, Пт: с 10-00 до 23-00 ч.
-Сб, Вс: с 09-00 до 23-00 ч.
-Мужские дни: Пн, Ср, Чт, Пт, Сб, Вс
-Женские дни: Вт</t>
-        </is>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Большая Марьинская улица, дом 1А </t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-CLUB SPACE - элитная сауна по приемлемым ценам в Москве,  расположена в Останкинском районе столицы,  недалеко от метро Алексеевская или Рижская.  
-Попадая в наш банный комплекс,  сразу погрузитесь в мир роскоши,  расслабления,  первоклассного сервиса и гостеприимства. 
-Наша отличительная черта - уважение к вашему комфорту,  конфиденциальности и приватности. 
-В сауне CLUB SPACE три отделения,  вместимостью от 8 до 40 человек.  Каждое отделение оборудовано всем необходимым для вашего банно-оздоровительного отдыха. 
-В сауне для гостей:
-Парная: финская и турецкая вместимостью до 10 человек каждая;
-Банные услуги: банщик,  выбор веников,  различные виды пропарок,  программы по телу,  турецкий пиллинг,  обертывания,  спа-терапия,  ароматерапия,  ароматы для парной;
-Комнаты отдыха: несколько комнат для отдыха и романтического свидания,  с уютной отделкой интерьера и двуспальными кроватями. 
-Зона отдыха и развлечения: гостиная,  банкетный зал,  кальян,  кальянная комната,  ассортимент табака,  сигары,  бар,  танцпол,  стрип-подиум,  стриптиз-шоу,  шоу программы,  аудио-видео аппаратура,  эротические каналы,  караоке,  бесплатный Wi-Fi;
-Кухня: домашняя,  русская,  европейская кухня,  бар с напитками;
-Бассейны: подогрев,  противоток,  фильтрация,  джакузи,  купель,  подсветка,  гейзер,  гидромассаж;
-Оздоровление: массажный стол,  оздоровительный массаж,  гидромассаж,  купель,  джакузи;
-Парковка клуба: бесплатная,  охраняемая парковка для наших гостей. 
-Зал "CITY SPACE" - самый вместительный из всех залов.  Используется для корпоративов,  встреч выпускников,  юбилеев и празднования других знаменательных событий в большой компании.  Для этого здесь имеется сцена с профессиональным оборудованием и караоке.  При желании,  мы можем украсить зал к вашему торжеству и пригласить артистов,  музыкантов или другие творческие коллективы.  Вмещает до 40 человек,  площадь зала 450 кв. м
-Зал "SMALL SPACE" - выделяется стильным интерьером.  Комнаты отдыха здесь обставлены и декорированы с большим вкусом.  Это помещение отлично подходит для отдыха в семейном кругу или для встреч с деловыми партнерами.  Вмещает до 20 человек,  площадь зала 220 кв. м
-Зал "NEW SPACE" - самый маленький и уютный зал,  отлично подойдет для проведения романтического свидания,  отдыха в кругу семьи или дружеских посиделок небольшой компании.  Вмещает до 8 человек,  площадь зала 80 кв. м
-Забронировать сауну или узнать подробную информации можете по телефону:
-+7 499 705 46 13
-Официальный сайт сауны:
-https://club-space24.ru/
-За сутки: 72
-За последние 30 дней: 184
-Всего: 6822
-</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Вид парной: финская парная, турецкая парная(хамам)Кухня: русская, бар, меню доставкиУслуги: веники, банщик, спа-терапия, оздоровительный массаж, ароматерапия, кальян, музыкальный центр, банкеты, оплата картамиСервис: бассейн, кондиционер, бильярд, охраняемая парковка, джакузи, холодная купель, спутниковое тв, караоке, Wi-Fi, обливное ведро, большой TV, бассейн с противотоком
-</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">СТОИМОСТЬ
-CITY SPACE (до 40 человек):
-- 5000 - 7000 руб/час;
-SMALL SPACE (до 20 человек):
-- 3000 - 4500 руб/час;
-NEW SPACE (до 8 человек):
-- 2000 - 3000 руб/час
- </t>
-        </is>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
v2 Add more filters and to export Excel
</commit_message>
<xml_diff>
--- a/output2.xlsx
+++ b/output2.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,9 +445,9 @@
 +7 985 795 07 56 
 или на официальном сайте банного комплекса "Time Park":
 https://time-park.ru/
-За сутки: 226
-За последние 30 дней: 336
-Всего: 2466
+За сутки: 262
+За последние 30 дней: 372
+Всего: 2502
 </t>
         </is>
       </c>
@@ -470,6 +470,11 @@
       <c r="E1" t="b">
         <v>0</v>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>финская парная, русская баня, русская на дровах</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>